<commit_message>
pilot 1: subject 1 + subject 2
</commit_message>
<xml_diff>
--- a/data_analysis/pilot_1/pilot1_subjects.xlsx
+++ b/data_analysis/pilot_1/pilot1_subjects.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67E5025D-BB11-4735-B2CC-50D4A8FE1A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{67E5025D-BB11-4735-B2CC-50D4A8FE1A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2736E42-B33D-44B9-854D-8C4FC8363295}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Elenco inventario'!#REF!</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Elenco inventario'!$1:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Elenco inventario'!$1:$1</definedName>
     <definedName name="valHighlight">IFERROR(IF('Elenco inventario'!#REF!="Sì", TRUE, FALSE),FALSE)</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>SUBJECT NUMBER</t>
   </si>
@@ -44,25 +44,41 @@
     <t>SEX</t>
   </si>
   <si>
-    <t>START TIME</t>
+    <t>COMMENTS</t>
   </si>
   <si>
-    <t>END TIME</t>
+    <t>M</t>
   </si>
   <si>
-    <t>TUTORIAL DURATION</t>
+    <t>TUTORIAL DURATION (minutes)</t>
+  </si>
+  <si>
+    <t>LINK SENT</t>
+  </si>
+  <si>
+    <t>EXP ERIMENT COMPLETED</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>it was not clear that the shuffles were starting from zero at every trial, so at the beginning he was trying to use as few as possible -&gt; underline it more during the tutorial with feedback</t>
+  </si>
+  <si>
+    <t>bad quality images during tutorial (no feedback) + thought that using more shuffles resulted in more difficult following trials</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="&quot;€&quot;\ #,##0.00"/>
+    <numFmt numFmtId="168" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -555,7 +571,6 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -563,13 +578,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
@@ -577,14 +586,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -636,7 +654,7 @@
     <cellStyle name="Valuta" xfId="3" builtinId="4" customBuiltin="1"/>
     <cellStyle name="Valuta [0]" xfId="4" builtinId="7" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="21">
     <dxf>
       <font>
         <b val="0"/>
@@ -654,6 +672,54 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="168" formatCode="h:mm;@"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="h:mm;@"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="166" formatCode="&quot;€&quot;\ #,##0.00"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -676,19 +742,6 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="1" tint="0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -740,7 +793,11 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -750,7 +807,6 @@
         <name val="Franklin Gothic Book"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="&quot;€&quot;\ #,##0.00"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -948,9 +1004,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Tabella Aziendale" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="18"/>
-      <tableStyleElement type="headerRow" dxfId="17"/>
-      <tableStyleElement type="secondRowStripe" dxfId="16"/>
+      <tableStyleElement type="wholeTable" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="19"/>
+      <tableStyleElement type="secondRowStripe" dxfId="18"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -965,15 +1021,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella_Elenco_inventario" displayName="Tabella_Elenco_inventario" ref="B3:G28" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="B3:G28" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SUBJECT NUMBER" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="AGE" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SEX" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="START TIME" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="1" xr3:uid="{CD4CDB13-532F-4C56-A86A-6B439CF29546}" name="END TIME" dataDxfId="0" totalsRowDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="TUTORIAL DURATION" dataDxfId="5" totalsRowDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella_Elenco_inventario" displayName="Tabella_Elenco_inventario" ref="B1:H26" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="B1:H26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="7">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SUBJECT NUMBER" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="AGE" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SEX" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="LINK SENT" dataDxfId="1" totalsRowDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{CD4CDB13-532F-4C56-A86A-6B439CF29546}" name="EXP ERIMENT COMPLETED" dataDxfId="0" totalsRowDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{9E08D108-5F48-4257-A8B1-A9E4D6B05F3D}" name="TUTORIAL DURATION (minutes)" dataDxfId="4" totalsRowDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="COMMENTS" dataDxfId="7" totalsRowDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="Tabella Aziendale" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1182,158 +1239,164 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G28"/>
+  <dimension ref="B1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.81640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" style="5" customWidth="1"/>
-    <col min="3" max="4" width="16.81640625" style="5" customWidth="1"/>
-    <col min="5" max="7" width="12.90625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="1.81640625" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="8.81640625" style="3"/>
+    <col min="1" max="1" width="1.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" style="3" customWidth="1"/>
+    <col min="3" max="4" width="16.81640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="12.90625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="12.90625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="44.1796875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="1.81640625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="1" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="2:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="10"/>
-    </row>
-    <row r="3" spans="2:7" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="8" t="s">
+    <row r="1" spans="2:8" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="8" t="s">
+    </row>
+    <row r="2" spans="2:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-    </row>
-    <row r="5" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-    </row>
-    <row r="6" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-    </row>
-    <row r="12" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" spans="5:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="5:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" spans="5:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-    </row>
-    <row r="20" spans="5:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" spans="5:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="5:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="5:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24" spans="5:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" spans="5:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-    </row>
-    <row r="26" spans="5:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-    </row>
-    <row r="27" spans="5:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-    </row>
-    <row r="28" spans="5:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
+      <c r="E2" s="10">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="F2" s="10">
+        <v>0.4458333333333333</v>
+      </c>
+      <c r="G2" s="8">
+        <v>11</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>24</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0.4770833333333333</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0.49861111111111112</v>
+      </c>
+      <c r="G3" s="8">
+        <v>13</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G22" s="6"/>
+    </row>
+    <row r="23" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G26" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B4:G28">
+  <conditionalFormatting sqref="B2:H26">
     <cfRule type="expression" dxfId="3" priority="8">
       <formula>#REF!="Sì"</formula>
     </cfRule>
@@ -1341,14 +1404,12 @@
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="67" yWindow="628" count="7">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Elenco inventario" prompt="_x000a_Il foglio di lavoro traccia l'inventario degli articoli in Elenco inventario e consente di contrassegnare quelli che è possibile riordinare. Gli articoli fuori produzione hanno il formato barrato e il testo Sì nella colonna Fuori produzione." sqref="A2" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere l'ID inventario in questa colonna" sqref="B3" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'articolo in questa colonna" sqref="C3" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la quantità in magazzino di ogni articolo in questa colonna" sqref="G3" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il prezzo unitario di ogni articolo in questa colonna" sqref="E3:F3" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere una descrizione dell'articolo in questa colonna" sqref="D3" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Elenco inventario" prompt="Il foglio di lavoro traccia l'inventario degli articoli in Elenco inventario e consente di contrassegnare quelli che è possibile riordinare. Gli articoli fuori produzione hanno il formato barrato e il testo Sì nella colonna Fuori produzione." sqref="A1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+  <dataValidations xWindow="67" yWindow="628" count="5">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere l'ID inventario in questa colonna" sqref="B1" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'articolo in questa colonna" sqref="C1" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la quantità in magazzino di ogni articolo in questa colonna" sqref="H1" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il prezzo unitario di ogni articolo in questa colonna" sqref="E1:G1" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere una descrizione dell'articolo in questa colonna" sqref="D1" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="52" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -1359,21 +1420,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1585,19 +1646,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
subject 3 data uploaded
</commit_message>
<xml_diff>
--- a/data_analysis/pilot_1/pilot1_subjects.xlsx
+++ b/data_analysis/pilot_1/pilot1_subjects.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{67E5025D-BB11-4735-B2CC-50D4A8FE1A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2736E42-B33D-44B9-854D-8C4FC8363295}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="8_{67E5025D-BB11-4735-B2CC-50D4A8FE1A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E916104-BD0D-4346-BC5C-0657453D704A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>SUBJECT NUMBER</t>
   </si>
@@ -62,23 +62,25 @@
     <t>F</t>
   </si>
   <si>
-    <t>it was not clear that the shuffles were starting from zero at every trial, so at the beginning he was trying to use as few as possible -&gt; underline it more during the tutorial with feedback</t>
+    <t>bad quality images during tutorial (no feedback) + thought that using more shuffles resulted in more difficult following trials</t>
   </si>
   <si>
-    <t>bad quality images during tutorial (no feedback) + thought that using more shuffles resulted in more difficult following trials</t>
+    <t>when starting tutorial (no feedback), she was expecting to see the red version first (it is the first time the black one is shown first)  + problems visualizing the text with Safari (version 14.1.1 ) + it's written "right or left" arrow, but instead it should be "left or right" + she did not feel tired at all, could have done other 2/3 blocks</t>
+  </si>
+  <si>
+    <t>it was not clear that the shuffles were starting from zero at every trial, so at the beginning he was trying to use as few as possible -&gt; underline it more during the tutorial with feedback + safari version 16.4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="&quot;€&quot;\ #,##0.00"/>
-    <numFmt numFmtId="168" formatCode="h:mm;@"/>
+    <numFmt numFmtId="167" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -569,7 +571,7 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -586,23 +588,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -672,7 +671,38 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="168" formatCode="h:mm;@"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -687,21 +717,43 @@
         <name val="Franklin Gothic Book"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="168" formatCode="h:mm;@"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="1" tint="0.34998626667073579"/>
-      </font>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -720,7 +772,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="&quot;€&quot;\ #,##0.00"/>
+      <numFmt numFmtId="167" formatCode="h:mm;@"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -743,24 +795,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Franklin Gothic Book"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -771,42 +805,7 @@
         <name val="Franklin Gothic Book"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Franklin Gothic Book"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Franklin Gothic Book"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="167" formatCode="h:mm;@"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1020,6 +1019,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella_Elenco_inventario" displayName="Tabella_Elenco_inventario" ref="B1:H26" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="B1:H26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
@@ -1027,10 +1030,10 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SUBJECT NUMBER" dataDxfId="15" totalsRowDxfId="14"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="AGE" dataDxfId="13" totalsRowDxfId="12"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SEX" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="LINK SENT" dataDxfId="1" totalsRowDxfId="9"/>
-    <tableColumn id="1" xr3:uid="{CD4CDB13-532F-4C56-A86A-6B439CF29546}" name="EXP ERIMENT COMPLETED" dataDxfId="0" totalsRowDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{9E08D108-5F48-4257-A8B1-A9E4D6B05F3D}" name="TUTORIAL DURATION (minutes)" dataDxfId="4" totalsRowDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="COMMENTS" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="LINK SENT" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{CD4CDB13-532F-4C56-A86A-6B439CF29546}" name="EXP ERIMENT COMPLETED" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{9E08D108-5F48-4257-A8B1-A9E4D6B05F3D}" name="TUTORIAL DURATION (minutes)" dataDxfId="0" totalsRowDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="COMMENTS" dataDxfId="4" totalsRowDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="Tabella Aziendale" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1239,10 +1242,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H26"/>
+  <dimension ref="B1:H5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1250,8 +1253,8 @@
     <col min="1" max="1" width="1.81640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.81640625" style="3" customWidth="1"/>
     <col min="3" max="4" width="16.81640625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="12.90625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="12.90625" style="4" customWidth="1"/>
+    <col min="5" max="6" width="12.90625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="12.90625" style="10" customWidth="1"/>
     <col min="8" max="8" width="44.1796875" style="4" customWidth="1"/>
     <col min="9" max="9" width="1.81640625" style="2" customWidth="1"/>
     <col min="10" max="16384" width="8.81640625" style="2"/>
@@ -1267,20 +1270,20 @@
       <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="49.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="3">
         <v>1</v>
       </c>
@@ -1290,17 +1293,17 @@
       <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="7">
         <v>0.42708333333333331</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="7">
         <v>0.4458333333333333</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="10">
         <v>11</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>9</v>
+      <c r="H2" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
@@ -1313,94 +1316,62 @@
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="7">
         <v>0.4770833333333333</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="7">
         <v>0.49861111111111112</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="10">
         <v>13</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>26</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0.61319444444444449</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0.62638888888888888</v>
+      </c>
+      <c r="G4" s="10">
+        <v>12</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G19" s="6"/>
-    </row>
-    <row r="20" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G21" s="6"/>
-    </row>
-    <row r="22" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G22" s="6"/>
-    </row>
-    <row r="23" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G24" s="6"/>
-    </row>
-    <row r="25" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G25" s="6"/>
-    </row>
-    <row r="26" spans="7:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G26" s="6"/>
+      <c r="B5" s="3">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3">
+        <v>27</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0.60833333333333328</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:H26">
-    <cfRule type="expression" dxfId="3" priority="8">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>#REF!="Sì"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="9">
+    <cfRule type="expression" dxfId="1" priority="9">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1420,21 +1391,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1646,19 +1617,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
subject 4-5-6 data uploaded
</commit_message>
<xml_diff>
--- a/data_analysis/pilot_1/pilot1_subjects.xlsx
+++ b/data_analysis/pilot_1/pilot1_subjects.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="77" documentId="8_{67E5025D-BB11-4735-B2CC-50D4A8FE1A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E916104-BD0D-4346-BC5C-0657453D704A}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="8_{67E5025D-BB11-4735-B2CC-50D4A8FE1A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EC98541-6DB1-40E9-806C-871FC9E63D01}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>SUBJECT NUMBER</t>
   </si>
@@ -56,19 +56,28 @@
     <t>LINK SENT</t>
   </si>
   <si>
-    <t>EXP ERIMENT COMPLETED</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
-    <t>bad quality images during tutorial (no feedback) + thought that using more shuffles resulted in more difficult following trials</t>
+    <t>EXPERIMENT COMPLETED</t>
   </si>
   <si>
-    <t>when starting tutorial (no feedback), she was expecting to see the red version first (it is the first time the black one is shown first)  + problems visualizing the text with Safari (version 14.1.1 ) + it's written "right or left" arrow, but instead it should be "left or right" + she did not feel tired at all, could have done other 2/3 blocks</t>
+    <t xml:space="preserve">INSTRUCTIONS: 1. indicate which is the last page when it is possible to you can go back, before moving on with tutorial; 2. Avoid repeating same senteces over and over, since it is possible to go back; 3. Convey the idea that the task will become very difficult, with some difficult examples in the tutorial.  TASK: communicate score of last trial of block. </t>
   </si>
   <si>
-    <t>it was not clear that the shuffles were starting from zero at every trial, so at the beginning he was trying to use as few as possible -&gt; underline it more during the tutorial with feedback + safari version 16.4</t>
+    <t>TUTORIAL (I part): bad quality images during tutorial; TASK: thought that using more shuffles resulted in more difficult following trials</t>
+  </si>
+  <si>
+    <t>TASK: it was not clear that the shuffles were starting from zero at every trial, so at the beginning he was trying to use as few as possible -&gt; underline it more during the tutorial with feedback + safari version 16.4</t>
+  </si>
+  <si>
+    <t>TUTORIAL (I part): when starting tutorial, she was expecting to see the red version first (it is the first time the black one is shown first)  + BROWSER COMPATIBILITY: problems visualizing the text (FillText) with Safari (version 14.1.1 ) + it's written "right or left" arrow, but instead it should be "left or right" + she did not feel tired at all, could have done other 2/3 blocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTRO PAGE: change title (New Version of...) + you will receive INSTRUCTIONS…  + in case you HAVE QUESTIONS regarding + AND THAT of the other volunteers. BROWSER compatibility: (Firefox -&gt; informed consent page not fitting, is cut. Also score is cut during the task). TUTORIAL (II part): low quality of images. TASK: she was expecting to see the score after pressing spacebar, like in the tutorial (she suggested to make it more consistent in the two cases. Maybe by inverting the score increase - solution images). </t>
+  </si>
+  <si>
+    <t>TASK: it was not clear what shuffles meant, he was thinking that one space bar press randomized the graph, and another one was taking the graph back to the previous visualization. Was very fast, but could not handle one trial more. Maybe he misunderstood / did not read the instructions carefully enough.</t>
   </si>
 </sst>
 </file>
@@ -80,7 +89,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="h:mm;@"/>
+    <numFmt numFmtId="166" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -588,10 +597,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -655,6 +664,69 @@
   </cellStyles>
   <dxfs count="21">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -675,19 +747,6 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="1" tint="0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -707,7 +766,11 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -715,8 +778,10 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Franklin Gothic Book"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="166" formatCode="h:mm;@"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -739,62 +804,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Franklin Gothic Book"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="h:mm;@"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Franklin Gothic Book"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -805,7 +814,7 @@
         <name val="Franklin Gothic Book"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="h:mm;@"/>
+      <numFmt numFmtId="166" formatCode="h:mm;@"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1031,9 +1040,9 @@
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="AGE" dataDxfId="13" totalsRowDxfId="12"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SEX" dataDxfId="11" totalsRowDxfId="10"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="LINK SENT" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="1" xr3:uid="{CD4CDB13-532F-4C56-A86A-6B439CF29546}" name="EXP ERIMENT COMPLETED" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{9E08D108-5F48-4257-A8B1-A9E4D6B05F3D}" name="TUTORIAL DURATION (minutes)" dataDxfId="0" totalsRowDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="COMMENTS" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{CD4CDB13-532F-4C56-A86A-6B439CF29546}" name="EXPERIMENT COMPLETED" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{9E08D108-5F48-4257-A8B1-A9E4D6B05F3D}" name="TUTORIAL DURATION (minutes)" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="COMMENTS" dataDxfId="3" totalsRowDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="Tabella Aziendale" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1242,20 +1251,22 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H5"/>
+  <dimension ref="B1:H11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="1.81640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" style="3" customWidth="1"/>
-    <col min="3" max="4" width="16.81640625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="12.90625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="12.90625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="44.1796875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="5.90625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.08984375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="9" style="7" customWidth="1"/>
+    <col min="7" max="7" width="8.08984375" style="10" customWidth="1"/>
+    <col min="8" max="8" width="64.90625" style="4" customWidth="1"/>
     <col min="9" max="9" width="1.81640625" style="2" customWidth="1"/>
     <col min="10" max="16384" width="8.81640625" style="2"/>
   </cols>
@@ -1274,7 +1285,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>5</v>
@@ -1314,7 +1325,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="7">
         <v>0.4770833333333333</v>
@@ -1326,7 +1337,7 @@
         <v>13</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1337,7 +1348,7 @@
         <v>26</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="7">
         <v>0.61319444444444449</v>
@@ -1349,10 +1360,10 @@
         <v>12</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="49.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3">
         <v>4</v>
       </c>
@@ -1363,15 +1374,90 @@
         <v>4</v>
       </c>
       <c r="E5" s="7">
-        <v>0.60833333333333328</v>
+        <v>0.65</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.67638888888888893</v>
+      </c>
+      <c r="G5" s="10">
+        <v>10</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0.42152777777777778</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0.43611111111111112</v>
+      </c>
+      <c r="G6" s="10">
+        <v>9</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="64.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="3">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.45694444444444443</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.46388888888888885</v>
+      </c>
+      <c r="G7" s="10">
+        <v>5</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="3">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:H26">
-    <cfRule type="expression" dxfId="2" priority="8">
+    <cfRule type="expression" dxfId="1" priority="8">
       <formula>#REF!="Sì"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="9">
+    <cfRule type="expression" dxfId="0" priority="9">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1391,24 +1477,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DEEA25CC0A0AC24199CDC46C25B8B0BC" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3b47856d4cf355c0dacb39e1084d14f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6dc4bcd6-49db-4c07-9060-8acfc67cef9f" xmlns:ns3="fb0879af-3eba-417a-a55a-ffe6dcd6ca77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a845a615265fdb1f7b12cc65ac20ecbd" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1616,25 +1684,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1227E31-123E-44EE-A422-2705DF3A5917}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1652,4 +1720,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
subject 7 data uploaded
</commit_message>
<xml_diff>
--- a/data_analysis/pilot_1/pilot1_subjects.xlsx
+++ b/data_analysis/pilot_1/pilot1_subjects.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="142" documentId="8_{67E5025D-BB11-4735-B2CC-50D4A8FE1A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EC98541-6DB1-40E9-806C-871FC9E63D01}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="8_{67E5025D-BB11-4735-B2CC-50D4A8FE1A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BBFA063-802F-4862-93AD-75CC5341B8D0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>SUBJECT NUMBER</t>
   </si>
@@ -78,6 +78,21 @@
   </si>
   <si>
     <t>TASK: it was not clear what shuffles meant, he was thinking that one space bar press randomized the graph, and another one was taking the graph back to the previous visualization. Was very fast, but could not handle one trial more. Maybe he misunderstood / did not read the instructions carefully enough.</t>
+  </si>
+  <si>
+    <t>LAURA</t>
+  </si>
+  <si>
+    <t>CHIARA</t>
+  </si>
+  <si>
+    <t>COSTAS?</t>
+  </si>
+  <si>
+    <t>TOTAL DURATION (minutes)</t>
+  </si>
+  <si>
+    <t>TASK: she tried to be as fast as accurate and possible with no help, so she did not think of using the shuffles when she was unsure about the answer. Maybe one could underline more that there is no penalization in using the shuffles and that there is no time limit, and that shuffling helps in giving an answer. She could have handled 2 more blocks. NOTE: the internet connection was interrupted, so she had to restart the experiment. This is the reason for the fast execution of tutorial.</t>
   </si>
 </sst>
 </file>
@@ -91,7 +106,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +244,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -662,7 +683,45 @@
     <cellStyle name="Valuta" xfId="3" builtinId="4" customBuiltin="1"/>
     <cellStyle name="Valuta [0]" xfId="4" builtinId="7" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1012,9 +1071,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Tabella Aziendale" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="20"/>
-      <tableStyleElement type="headerRow" dxfId="19"/>
-      <tableStyleElement type="secondRowStripe" dxfId="18"/>
+      <tableStyleElement type="wholeTable" dxfId="22"/>
+      <tableStyleElement type="headerRow" dxfId="21"/>
+      <tableStyleElement type="secondRowStripe" dxfId="20"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1033,16 +1092,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella_Elenco_inventario" displayName="Tabella_Elenco_inventario" ref="B1:H26" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="B1:H26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="7">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SUBJECT NUMBER" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="AGE" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SEX" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="LINK SENT" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="1" xr3:uid="{CD4CDB13-532F-4C56-A86A-6B439CF29546}" name="EXPERIMENT COMPLETED" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{9E08D108-5F48-4257-A8B1-A9E4D6B05F3D}" name="TUTORIAL DURATION (minutes)" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="COMMENTS" dataDxfId="3" totalsRowDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella_Elenco_inventario" displayName="Tabella_Elenco_inventario" ref="B1:I26" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="B1:I26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="8">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SUBJECT NUMBER" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="AGE" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SEX" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="LINK SENT" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{CD4CDB13-532F-4C56-A86A-6B439CF29546}" name="EXPERIMENT COMPLETED" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{5B371E51-03B6-41D4-90E0-50994B74D049}" name="TOTAL DURATION (minutes)" dataDxfId="0" totalsRowDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{9E08D108-5F48-4257-A8B1-A9E4D6B05F3D}" name="TUTORIAL DURATION (minutes)" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="COMMENTS" dataDxfId="5" totalsRowDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="Tabella Aziendale" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1251,27 +1311,28 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H11"/>
+  <dimension ref="B1:I11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="1.81640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="5.90625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" style="3" customWidth="1"/>
     <col min="4" max="4" width="6.453125" style="3" customWidth="1"/>
     <col min="5" max="5" width="8.08984375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="9" style="7" customWidth="1"/>
-    <col min="7" max="7" width="8.08984375" style="10" customWidth="1"/>
-    <col min="8" max="8" width="64.90625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="1.81640625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.81640625" style="2"/>
+    <col min="6" max="6" width="11.81640625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="11.26953125" style="10" customWidth="1"/>
+    <col min="8" max="8" width="13.6328125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="85.26953125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="1.81640625" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:9" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1288,18 +1349,21 @@
         <v>8</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:8" ht="49.8" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" ht="49.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="C2" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>4</v>
@@ -1311,13 +1375,16 @@
         <v>0.4458333333333333</v>
       </c>
       <c r="G2" s="10">
+        <v>27</v>
+      </c>
+      <c r="H2" s="10">
         <v>11</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3">
         <v>2</v>
       </c>
@@ -1334,13 +1401,16 @@
         <v>0.49861111111111112</v>
       </c>
       <c r="G3" s="10">
+        <v>30</v>
+      </c>
+      <c r="H3" s="10">
         <v>13</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="3">
         <v>3</v>
       </c>
@@ -1357,13 +1427,16 @@
         <v>0.62638888888888888</v>
       </c>
       <c r="G4" s="10">
+        <v>18</v>
+      </c>
+      <c r="H4" s="10">
         <v>12</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="49.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" ht="49.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3">
         <v>4</v>
       </c>
@@ -1380,13 +1453,16 @@
         <v>0.67638888888888893</v>
       </c>
       <c r="G5" s="10">
+        <v>37</v>
+      </c>
+      <c r="H5" s="10">
         <v>10</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="I5" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3">
         <v>5</v>
       </c>
@@ -1403,13 +1479,16 @@
         <v>0.43611111111111112</v>
       </c>
       <c r="G6" s="10">
+        <v>20</v>
+      </c>
+      <c r="H6" s="10">
         <v>9</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="I6" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="64.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" ht="64.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="3">
         <v>6</v>
       </c>
@@ -1426,46 +1505,80 @@
         <v>0.46388888888888885</v>
       </c>
       <c r="G7" s="10">
+        <v>9</v>
+      </c>
+      <c r="H7" s="10">
         <v>5</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="I7" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="3">
         <v>7</v>
       </c>
+      <c r="C8" s="3">
+        <v>28</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0.48402777777777778</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.50069444444444444</v>
+      </c>
+      <c r="G8" s="10">
+        <v>6</v>
+      </c>
+      <c r="H8" s="10">
+        <v>3</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="9" spans="2:8" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="3">
         <v>8</v>
       </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="10" spans="2:8" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>9</v>
       </c>
+      <c r="C10" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="11" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>10</v>
       </c>
+      <c r="C11" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:H26">
-    <cfRule type="expression" dxfId="1" priority="8">
+  <phoneticPr fontId="19" type="noConversion"/>
+  <conditionalFormatting sqref="B2:I26">
+    <cfRule type="expression" dxfId="3" priority="8">
       <formula>#REF!="Sì"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="9">
+    <cfRule type="expression" dxfId="2" priority="9">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="67" yWindow="628" count="5">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere l'ID inventario in questa colonna" sqref="B1" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'articolo in questa colonna" sqref="C1" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la quantità in magazzino di ogni articolo in questa colonna" sqref="H1" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il prezzo unitario di ogni articolo in questa colonna" sqref="E1:G1" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la quantità in magazzino di ogni articolo in questa colonna" sqref="I1" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il prezzo unitario di ogni articolo in questa colonna" sqref="E1:H1" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere una descrizione dell'articolo in questa colonna" sqref="D1" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1477,6 +1590,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DEEA25CC0A0AC24199CDC46C25B8B0BC" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3b47856d4cf355c0dacb39e1084d14f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6dc4bcd6-49db-4c07-9060-8acfc67cef9f" xmlns:ns3="fb0879af-3eba-417a-a55a-ffe6dcd6ca77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a845a615265fdb1f7b12cc65ac20ecbd" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1684,25 +1815,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1227E31-123E-44EE-A422-2705DF3A5917}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1720,22 +1851,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
subjects 8-9-10 data uploaded
</commit_message>
<xml_diff>
--- a/data_analysis/pilot_1/pilot1_subjects.xlsx
+++ b/data_analysis/pilot_1/pilot1_subjects.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="184" documentId="8_{67E5025D-BB11-4735-B2CC-50D4A8FE1A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BBFA063-802F-4862-93AD-75CC5341B8D0}"/>
+  <xr:revisionPtr revIDLastSave="235" documentId="8_{67E5025D-BB11-4735-B2CC-50D4A8FE1A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B2B41EB-3385-4F36-B50B-9D2A8BD6AF29}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>SUBJECT NUMBER</t>
   </si>
@@ -80,19 +80,28 @@
     <t>TASK: it was not clear what shuffles meant, he was thinking that one space bar press randomized the graph, and another one was taking the graph back to the previous visualization. Was very fast, but could not handle one trial more. Maybe he misunderstood / did not read the instructions carefully enough.</t>
   </si>
   <si>
-    <t>LAURA</t>
-  </si>
-  <si>
-    <t>CHIARA</t>
-  </si>
-  <si>
-    <t>COSTAS?</t>
-  </si>
-  <si>
     <t>TOTAL DURATION (minutes)</t>
   </si>
   <si>
     <t>TASK: she tried to be as fast as accurate and possible with no help, so she did not think of using the shuffles when she was unsure about the answer. Maybe one could underline more that there is no penalization in using the shuffles and that there is no time limit, and that shuffling helps in giving an answer. She could have handled 2 more blocks. NOTE: the internet connection was interrupted, so she had to restart the experiment. This is the reason for the fast execution of tutorial.</t>
+  </si>
+  <si>
+    <t>25? Sasha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F </t>
+  </si>
+  <si>
+    <t>INSTRUCTIONS: she had a feeling that at a point she got the point, the instructions could have been a bit shorter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTRO PAGE: privacy (servers located in EU = the ones of SISSA?) + also in case results WILL/WOULD BE PUBLISHED. Data will be handled according to EU REGULATION. Space after "GDPR". Dot after following sentence. INSTRUCTIONS: 1. using the same color for highlighted rows and a different one for columns? 2. Square-triangle transition: let's cover A PART (not a half) of the square. 3. Using "..." between shaded and fully covered part. 4. A dot is missing in this part. 4. Switching two rows and columns TRANSFORMS the original triangle. 5. Vertical triangle (pointing right for the first time) -&gt; let's consider a FLIPPED VERSION of the inital triangle. 6. Ricontrolla di aver usato "regular checkerboard" o "chessboard" quando sono scacchiere regolari. 7. (shuffle in non-regular checkerboard) ALSO IN THIS CASE, a shuffle is the... 8. It is also possible to shuffle TRIANGLES WITH MORE TILES (not bigger). 9. ALSO IN THE CASE OF MORE TILES; a shuffle is the... 10. Lower the number of examples of shuffles with red clique (to make the tutorial faster)? 11. THE TRIANGLES OF THE EXPERIMENT WILL LOOK LIKE THIS (not "this will be the size of the bigger triangle...") 12. "One on the left... and one on the right" -&gt; non far sparire il triangolo di sx quando si mostra quello di destra (risparmio anche di un'immagine. Se possibile, cerca anche di far apparire i cambiamenti sui triangoli allineati) TUTORIAL (pt. 2): "shuffles are limited" is repeated twice. 2. Organizza come: SHUFFLE 1 - SHUFFLE 2 - SHUFFLE 3 - FEEDBACK + SOLUZIONE (insieme, in modo che la visualizzazione successiva sia il trial successivo). 3. Sottolineare il fatto che nel task ci saranno più trials (dire proprio il numero -&gt; "you will have ... shuffles for each couple of graphs"). FINAL CONSENT: "consent" or "consense"? Centrare l'elenco, ma non mettere i punti su linee diverse. TASK: 1. suggest to wear glasses at the beginning? 2. Feedback between blocks -&gt; elenco puntato non centrato. 3. Decrease number of shuffles 4. Inter-trial interval più lungo per evitare sensory memory/after effect. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HINT: maybe one could underline the fact that the task will become more and more difficult and that the shuffles particularly helpful in more difficult trials. </t>
+  </si>
+  <si>
+    <t>INSTRUCTIONS: on Safari, "INSTRUCTIONS" is not centered in the screen. Possibility: using the same color for highlighted rows and a different one for columns? TASK: She was expecting to see red tiles appear after giving an answer</t>
   </si>
 </sst>
 </file>
@@ -601,7 +610,7 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -632,6 +641,12 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -685,6 +700,69 @@
   </cellStyles>
   <dxfs count="23">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -702,69 +780,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Franklin Gothic Book"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="1" tint="0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Franklin Gothic Book"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Franklin Gothic Book"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1100,9 +1115,9 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SEX" dataDxfId="13" totalsRowDxfId="12"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="LINK SENT" dataDxfId="11" totalsRowDxfId="10"/>
     <tableColumn id="1" xr3:uid="{CD4CDB13-532F-4C56-A86A-6B439CF29546}" name="EXPERIMENT COMPLETED" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{5B371E51-03B6-41D4-90E0-50994B74D049}" name="TOTAL DURATION (minutes)" dataDxfId="0" totalsRowDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{9E08D108-5F48-4257-A8B1-A9E4D6B05F3D}" name="TUTORIAL DURATION (minutes)" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="COMMENTS" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{5B371E51-03B6-41D4-90E0-50994B74D049}" name="TOTAL DURATION (minutes)" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{9E08D108-5F48-4257-A8B1-A9E4D6B05F3D}" name="TUTORIAL DURATION (minutes)" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="COMMENTS" dataDxfId="3" totalsRowDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="Tabella Aziendale" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1311,10 +1326,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:I11"/>
+  <dimension ref="B1:I13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1327,7 +1342,7 @@
     <col min="6" max="6" width="11.81640625" style="7" customWidth="1"/>
     <col min="7" max="7" width="11.26953125" style="10" customWidth="1"/>
     <col min="8" max="8" width="13.6328125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="85.26953125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="117.08984375" style="4" customWidth="1"/>
     <col min="10" max="10" width="1.81640625" style="2" customWidth="1"/>
     <col min="11" max="16384" width="8.81640625" style="2"/>
   </cols>
@@ -1349,7 +1364,7 @@
         <v>8</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>5</v>
@@ -1359,25 +1374,25 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="49.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1">
         <v>28</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="11">
         <v>0.42708333333333331</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="11">
         <v>0.4458333333333333</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="12">
         <v>27</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="12">
         <v>11</v>
       </c>
       <c r="I2" s="8" t="s">
@@ -1385,25 +1400,25 @@
       </c>
     </row>
     <row r="3" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <v>24</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="11">
         <v>0.4770833333333333</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="11">
         <v>0.49861111111111112</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="12">
         <v>30</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="12">
         <v>13</v>
       </c>
       <c r="I3" s="8" t="s">
@@ -1411,25 +1426,25 @@
       </c>
     </row>
     <row r="4" spans="2:9" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <v>26</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="11">
         <v>0.61319444444444449</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="11">
         <v>0.62638888888888888</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="12">
         <v>18</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="12">
         <v>12</v>
       </c>
       <c r="I4" s="8" t="s">
@@ -1437,25 +1452,25 @@
       </c>
     </row>
     <row r="5" spans="2:9" ht="49.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>27</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="11">
         <v>0.65</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="11">
         <v>0.67638888888888893</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="12">
         <v>37</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="12">
         <v>10</v>
       </c>
       <c r="I5" s="8" t="s">
@@ -1463,25 +1478,25 @@
       </c>
     </row>
     <row r="6" spans="2:9" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="3">
+      <c r="B6" s="1">
         <v>5</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
         <v>23</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="11">
         <v>0.42152777777777778</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="11">
         <v>0.43611111111111112</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="12">
         <v>20</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="12">
         <v>9</v>
       </c>
       <c r="I6" s="8" t="s">
@@ -1489,25 +1504,25 @@
       </c>
     </row>
     <row r="7" spans="2:9" ht="64.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <v>6</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <v>24</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="11">
         <v>0.45694444444444443</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="11">
         <v>0.46388888888888885</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="12">
         <v>9</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="12">
         <v>5</v>
       </c>
       <c r="I7" s="8" t="s">
@@ -1515,62 +1530,103 @@
       </c>
     </row>
     <row r="8" spans="2:9" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="3">
+      <c r="B8" s="1">
         <v>7</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1">
         <v>28</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="11">
         <v>0.48402777777777778</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="11">
         <v>0.50069444444444444</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="12">
         <v>6</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="12">
         <v>3</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="3">
+      <c r="B9" s="1">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>15</v>
+      <c r="C9" s="1">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.66597222222222219</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0.69236111111111109</v>
+      </c>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="3">
+      <c r="B10" s="1">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>16</v>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0.68958333333333333</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="8" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="3">
+    <row r="11" spans="2:9" ht="174" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="1">
         <v>10</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>17</v>
+      <c r="C11" s="1">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I13" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <conditionalFormatting sqref="B2:I26">
-    <cfRule type="expression" dxfId="3" priority="8">
+    <cfRule type="expression" dxfId="1" priority="8">
       <formula>#REF!="Sì"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="9">
+    <cfRule type="expression" dxfId="0" priority="9">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1590,24 +1646,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DEEA25CC0A0AC24199CDC46C25B8B0BC" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3b47856d4cf355c0dacb39e1084d14f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6dc4bcd6-49db-4c07-9060-8acfc67cef9f" xmlns:ns3="fb0879af-3eba-417a-a55a-ffe6dcd6ca77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a845a615265fdb1f7b12cc65ac20ecbd" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1815,25 +1853,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1227E31-123E-44EE-A422-2705DF3A5917}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1851,4 +1889,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated subjects xlsx file for pilot 1
</commit_message>
<xml_diff>
--- a/data_analysis/pilot_1/pilot1_subjects.xlsx
+++ b/data_analysis/pilot_1/pilot1_subjects.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="235" documentId="8_{67E5025D-BB11-4735-B2CC-50D4A8FE1A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B2B41EB-3385-4F36-B50B-9D2A8BD6AF29}"/>
+  <xr:revisionPtr revIDLastSave="248" documentId="8_{67E5025D-BB11-4735-B2CC-50D4A8FE1A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F9014E5-68EC-4271-9999-1BDEC5047666}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>SUBJECT NUMBER</t>
   </si>
@@ -86,9 +86,6 @@
     <t>TASK: she tried to be as fast as accurate and possible with no help, so she did not think of using the shuffles when she was unsure about the answer. Maybe one could underline more that there is no penalization in using the shuffles and that there is no time limit, and that shuffling helps in giving an answer. She could have handled 2 more blocks. NOTE: the internet connection was interrupted, so she had to restart the experiment. This is the reason for the fast execution of tutorial.</t>
   </si>
   <si>
-    <t>25? Sasha</t>
-  </si>
-  <si>
     <t xml:space="preserve">F </t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>INSTRUCTIONS: on Safari, "INSTRUCTIONS" is not centered in the screen. Possibility: using the same color for highlighted rows and a different one for columns? TASK: She was expecting to see red tiles appear after giving an answer</t>
+  </si>
+  <si>
+    <t>(pauses within experiment)</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,7 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -647,6 +647,9 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -1328,8 +1331,8 @@
   </sheetPr>
   <dimension ref="B1:I13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1571,18 +1574,22 @@
       <c r="F9" s="11">
         <v>0.69236111111111109</v>
       </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
+      <c r="G9" s="12">
+        <v>31</v>
+      </c>
+      <c r="H9" s="12">
+        <v>12</v>
+      </c>
       <c r="I9" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1">
         <v>9</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>17</v>
+      <c r="C10" s="1">
+        <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
@@ -1590,11 +1597,17 @@
       <c r="E10" s="11">
         <v>0.68958333333333333</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+      <c r="F10" s="11">
+        <v>0.70624999999999993</v>
+      </c>
+      <c r="G10" s="12">
+        <v>23</v>
+      </c>
+      <c r="H10" s="12">
+        <v>12</v>
+      </c>
       <c r="I10" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="174" customHeight="1" x14ac:dyDescent="0.35">
@@ -1605,19 +1618,27 @@
         <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
+        <v>17</v>
+      </c>
+      <c r="E11" s="11">
+        <v>0.70972222222222225</v>
+      </c>
+      <c r="F11" s="11">
+        <v>0.7631944444444444</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>22</v>
+      </c>
       <c r="I11" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="I13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created pilot 1 feedbacks docx file
</commit_message>
<xml_diff>
--- a/data_analysis/pilot_1/pilot1_subjects.xlsx
+++ b/data_analysis/pilot_1/pilot1_subjects.xlsx
@@ -3,17 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="248" documentId="8_{67E5025D-BB11-4735-B2CC-50D4A8FE1A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F9014E5-68EC-4271-9999-1BDEC5047666}"/>
+  <xr:revisionPtr revIDLastSave="288" documentId="8_{67E5025D-BB11-4735-B2CC-50D4A8FE1A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCEA0430-C46E-41EA-80DB-6265537C42EC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Elenco inventario" sheetId="1" r:id="rId1"/>
+    <sheet name="Subjects" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Elenco inventario'!#REF!</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Elenco inventario'!$1:$1</definedName>
-    <definedName name="valHighlight">IFERROR(IF('Elenco inventario'!#REF!="Sì", TRUE, FALSE),FALSE)</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Subjects!#REF!</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Subjects!$1:$1</definedName>
+    <definedName name="valHighlight">IFERROR(IF(Subjects!#REF!="Sì", TRUE, FALSE),FALSE)</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>SUBJECT NUMBER</t>
   </si>
@@ -62,46 +62,417 @@
     <t>EXPERIMENT COMPLETED</t>
   </si>
   <si>
-    <t xml:space="preserve">INSTRUCTIONS: 1. indicate which is the last page when it is possible to you can go back, before moving on with tutorial; 2. Avoid repeating same senteces over and over, since it is possible to go back; 3. Convey the idea that the task will become very difficult, with some difficult examples in the tutorial.  TASK: communicate score of last trial of block. </t>
-  </si>
-  <si>
-    <t>TUTORIAL (I part): bad quality images during tutorial; TASK: thought that using more shuffles resulted in more difficult following trials</t>
-  </si>
-  <si>
-    <t>TASK: it was not clear that the shuffles were starting from zero at every trial, so at the beginning he was trying to use as few as possible -&gt; underline it more during the tutorial with feedback + safari version 16.4</t>
-  </si>
-  <si>
-    <t>TUTORIAL (I part): when starting tutorial, she was expecting to see the red version first (it is the first time the black one is shown first)  + BROWSER COMPATIBILITY: problems visualizing the text (FillText) with Safari (version 14.1.1 ) + it's written "right or left" arrow, but instead it should be "left or right" + she did not feel tired at all, could have done other 2/3 blocks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INTRO PAGE: change title (New Version of...) + you will receive INSTRUCTIONS…  + in case you HAVE QUESTIONS regarding + AND THAT of the other volunteers. BROWSER compatibility: (Firefox -&gt; informed consent page not fitting, is cut. Also score is cut during the task). TUTORIAL (II part): low quality of images. TASK: she was expecting to see the score after pressing spacebar, like in the tutorial (she suggested to make it more consistent in the two cases. Maybe by inverting the score increase - solution images). </t>
-  </si>
-  <si>
-    <t>TASK: it was not clear what shuffles meant, he was thinking that one space bar press randomized the graph, and another one was taking the graph back to the previous visualization. Was very fast, but could not handle one trial more. Maybe he misunderstood / did not read the instructions carefully enough.</t>
-  </si>
-  <si>
     <t>TOTAL DURATION (minutes)</t>
-  </si>
-  <si>
-    <t>TASK: she tried to be as fast as accurate and possible with no help, so she did not think of using the shuffles when she was unsure about the answer. Maybe one could underline more that there is no penalization in using the shuffles and that there is no time limit, and that shuffling helps in giving an answer. She could have handled 2 more blocks. NOTE: the internet connection was interrupted, so she had to restart the experiment. This is the reason for the fast execution of tutorial.</t>
   </si>
   <si>
     <t xml:space="preserve">F </t>
   </si>
   <si>
-    <t>INSTRUCTIONS: she had a feeling that at a point she got the point, the instructions could have been a bit shorter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INTRO PAGE: privacy (servers located in EU = the ones of SISSA?) + also in case results WILL/WOULD BE PUBLISHED. Data will be handled according to EU REGULATION. Space after "GDPR". Dot after following sentence. INSTRUCTIONS: 1. using the same color for highlighted rows and a different one for columns? 2. Square-triangle transition: let's cover A PART (not a half) of the square. 3. Using "..." between shaded and fully covered part. 4. A dot is missing in this part. 4. Switching two rows and columns TRANSFORMS the original triangle. 5. Vertical triangle (pointing right for the first time) -&gt; let's consider a FLIPPED VERSION of the inital triangle. 6. Ricontrolla di aver usato "regular checkerboard" o "chessboard" quando sono scacchiere regolari. 7. (shuffle in non-regular checkerboard) ALSO IN THIS CASE, a shuffle is the... 8. It is also possible to shuffle TRIANGLES WITH MORE TILES (not bigger). 9. ALSO IN THE CASE OF MORE TILES; a shuffle is the... 10. Lower the number of examples of shuffles with red clique (to make the tutorial faster)? 11. THE TRIANGLES OF THE EXPERIMENT WILL LOOK LIKE THIS (not "this will be the size of the bigger triangle...") 12. "One on the left... and one on the right" -&gt; non far sparire il triangolo di sx quando si mostra quello di destra (risparmio anche di un'immagine. Se possibile, cerca anche di far apparire i cambiamenti sui triangoli allineati) TUTORIAL (pt. 2): "shuffles are limited" is repeated twice. 2. Organizza come: SHUFFLE 1 - SHUFFLE 2 - SHUFFLE 3 - FEEDBACK + SOLUZIONE (insieme, in modo che la visualizzazione successiva sia il trial successivo). 3. Sottolineare il fatto che nel task ci saranno più trials (dire proprio il numero -&gt; "you will have ... shuffles for each couple of graphs"). FINAL CONSENT: "consent" or "consense"? Centrare l'elenco, ma non mettere i punti su linee diverse. TASK: 1. suggest to wear glasses at the beginning? 2. Feedback between blocks -&gt; elenco puntato non centrato. 3. Decrease number of shuffles 4. Inter-trial interval più lungo per evitare sensory memory/after effect. </t>
-  </si>
-  <si>
     <t xml:space="preserve">HINT: maybe one could underline the fact that the task will become more and more difficult and that the shuffles particularly helpful in more difficult trials. </t>
   </si>
   <si>
-    <t>INSTRUCTIONS: on Safari, "INSTRUCTIONS" is not centered in the screen. Possibility: using the same color for highlighted rows and a different one for columns? TASK: She was expecting to see red tiles appear after giving an answer</t>
+    <t>(pauses within experiment)</t>
   </si>
   <si>
-    <t>(pauses within experiment)</t>
+    <t>KEY POINT: instruction information is not really used by the participants</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TASK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: not clear that the shuffles were re-starting from zero at every couple of graphs (he thought that they were 20 for each couple of graphs) [Safari version 16.4]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TUTORIAL (I part)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: when starting tutorial, she was expecting to see the red version first (it is the first time the black one is shown first)  + BROWSER COMPATIBILITY: problems visualizing the text (FillText) with Safari (version 14.1.1 ) + it's written "right or left" arrow, but instead it should be "left or right" + she did not feel tired at all, could have done other 2/3 blocks</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSTRUCTIONS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 1. indicate which is the last page when it is possible to you can go back, before moving on with tutorial; 2. Avoid repeating same senteces over and over, since it is possible to go back; 3. Convey the idea that the task will become very difficult, with some difficult examples in the tutorial.  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">TASK: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">communicate score of last trial of block. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TUTORIAL (I part)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: bad quality images during tutorial; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TASK:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> thought that using more shuffles resulted in more difficult following trials</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">TASK: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>it was not clear what shuffles meant, he was thinking that one space bar press randomized the graph, and another one was taking the graph back to the previous visualization. Was very fast, but could not handle one trial more. Maybe he misunderstood / did not read the instructions carefully enough.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TASK:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> she tried to be as fast as accurate and possible with no help, so she did not think of using the shuffles when she was unsure about the answer. Maybe one could underline more that there is no penalization in using the shuffles and that there is no time limit, and that shuffling helps in giving an answer. She could have handled 2 more blocks. NOTE: the internet connection was interrupted, so she had to restart the experiment. This is the reason for the fast execution of tutorial.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSTRUCTIONS:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> she had a feeling that at a point she got the point, the instructions could have been a bit shorter, especially in the part about the shuffles. Also at the beginning, maybe it was not necessary to move from the squares to triangles (going directly to explain the shuffles)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSTRUCTIONS:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on Safari, "INSTRUCTIONS" is not centered in the screen. Possibility: using the same color for highlighted rows and a different one for columns? </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">TASK: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>She was expecting to see red tiles appear after giving an answer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INTRO PAGE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: privacy (servers located in EU = the ones of SISSA?) + also in case results WILL/WOULD BE PUBLISHED. Data will be handled according to EU REGULATION. Space after "GDPR". Dot after following sentence.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> INSTRUCTIONS:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1. using the same color for highlighted rows and a different one for columns? 2. Square-triangle transition: let's cover A PART (not a half) of the square. 3. Using "..." between shaded and fully covered part. 4. A dot is missing in this part. 4. Switching two rows and columns TRANSFORMS the original triangle. 5. Vertical triangle (pointing right for the first time) -&gt; let's consider a FLIPPED VERSION of the inital triangle. 6. Ricontrolla di aver usato "regular checkerboard" o "chessboard" quando sono scacchiere regolari. 7. (shuffle in non-regular checkerboard) ALSO IN THIS CASE, a shuffle is the... 8. It is also possible to shuffle TRIANGLES WITH MORE TILES (not bigger). 9. ALSO IN THE CASE OF MORE TILES; a shuffle is the... 10. Lower the number of examples of shuffles with red clique (to make the tutorial faster)? 11. THE TRIANGLES OF THE EXPERIMENT WILL LOOK LIKE THIS (not "this will be the size of the bigger triangle...") 12. "One on the left... and one on the right" -&gt; non far sparire il triangolo di sx quando si mostra quello di destra (risparmio anche di un'immagine. Se possibile, cerca anche di far apparire i cambiamenti sui triangoli allineati) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TUTORIAL (pt. 2):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "shuffles are limited" is repeated twice. 2. Organizza come: SHUFFLE 1 - SHUFFLE 2 - SHUFFLE 3 - FEEDBACK + SOLUZIONE (insieme, in modo che la visualizzazione successiva sia il trial successivo). 3. Sottolineare il fatto che nel task ci saranno più trials (dire proprio il numero -&gt; "you will have ... shuffles for each couple of graphs"). FINAL CONSENT: "consent" or "consense"? Centrare l'elenco, ma non mettere i punti su linee diverse. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TASK:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1. suggest to wear glasses at the beginning? 2. Feedback between blocks -&gt; elenco puntato non centrato. 3. Decrease number of shuffles 4. Inter-trial interval più lungo per evitare sensory memory/after effect. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INTRO PAGE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: change title (New Version of...) + you will receive INSTRUCTIONS…  + in case you HAVE QUESTIONS regarding + AND THAT of the other volunteers. BROWSER compatibility: (Firefox -&gt; informed consent page not fitting, is cut. Also score is cut during the task).</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TUTORIAL (II part)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: low quality of images. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TASK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: she was expecting to see the score after pressing spacebar, like in the tutorial (she suggested to make it more consistent in the two cases. Maybe by inverting the score increase - solution images). </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -115,7 +486,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,6 +630,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1329,10 +1708,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:I13"/>
+  <dimension ref="B1:I14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1367,7 +1746,7 @@
         <v>8</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>5</v>
@@ -1399,7 +1778,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.35">
@@ -1425,7 +1804,7 @@
         <v>13</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1451,7 +1830,7 @@
         <v>12</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="49.2" customHeight="1" x14ac:dyDescent="0.35">
@@ -1477,7 +1856,7 @@
         <v>10</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="90" customHeight="1" x14ac:dyDescent="0.35">
@@ -1503,7 +1882,7 @@
         <v>9</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="64.2" customHeight="1" x14ac:dyDescent="0.35">
@@ -1529,7 +1908,7 @@
         <v>5</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -1555,7 +1934,7 @@
         <v>3</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
@@ -1581,7 +1960,7 @@
         <v>12</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
@@ -1610,7 +1989,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="174" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" ht="201.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1">
         <v>10</v>
       </c>
@@ -1618,7 +1997,7 @@
         <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E11" s="11">
         <v>0.70972222222222225</v>
@@ -1627,18 +2006,23 @@
         <v>0.7631944444444444</v>
       </c>
       <c r="G11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="I13" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I14" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1651,7 +2035,7 @@
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="67" yWindow="628" count="5">
+  <dataValidations xWindow="285" yWindow="468" count="5">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere l'ID inventario in questa colonna" sqref="B1" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'articolo in questa colonna" sqref="C1" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la quantità in magazzino di ogni articolo in questa colonna" sqref="I1" xr:uid="{00000000-0002-0000-0000-000009000000}"/>

</xml_diff>

<commit_message>
pilot 1: average block duration calculation
</commit_message>
<xml_diff>
--- a/data_analysis/pilot_1/pilot1_subjects.xlsx
+++ b/data_analysis/pilot_1/pilot1_subjects.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="288" documentId="8_{67E5025D-BB11-4735-B2CC-50D4A8FE1A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCEA0430-C46E-41EA-80DB-6265537C42EC}"/>
+  <xr:revisionPtr revIDLastSave="351" documentId="8_{67E5025D-BB11-4735-B2CC-50D4A8FE1A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B532D736-8449-4D95-905B-B212E0DDDD77}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>SUBJECT NUMBER</t>
   </si>
@@ -71,9 +71,6 @@
     <t xml:space="preserve">HINT: maybe one could underline the fact that the task will become more and more difficult and that the shuffles particularly helpful in more difficult trials. </t>
   </si>
   <si>
-    <t>(pauses within experiment)</t>
-  </si>
-  <si>
     <t>KEY POINT: instruction information is not really used by the participants</t>
   </si>
   <si>
@@ -473,6 +470,12 @@
       </rPr>
       <t xml:space="preserve">: she was expecting to see the score after pressing spacebar, like in the tutorial (she suggested to make it more consistent in the two cases. Maybe by inverting the score increase - solution images). </t>
     </r>
+  </si>
+  <si>
+    <t>AVERAGE BLOCK DURATION (minutes)</t>
+  </si>
+  <si>
+    <t>(pauses between blocks)</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1083,7 @@
     <cellStyle name="Valuta" xfId="3" builtinId="4" customBuiltin="1"/>
     <cellStyle name="Valuta [0]" xfId="4" builtinId="7" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="25">
     <dxf>
       <fill>
         <patternFill>
@@ -1093,6 +1096,44 @@
         <strike/>
         <color theme="1" tint="0.34998626667073579"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1468,9 +1509,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Tabella Aziendale" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="22"/>
-      <tableStyleElement type="headerRow" dxfId="21"/>
-      <tableStyleElement type="secondRowStripe" dxfId="20"/>
+      <tableStyleElement type="wholeTable" dxfId="24"/>
+      <tableStyleElement type="headerRow" dxfId="23"/>
+      <tableStyleElement type="secondRowStripe" dxfId="22"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1489,17 +1530,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella_Elenco_inventario" displayName="Tabella_Elenco_inventario" ref="B1:I26" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="B1:I26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="8">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SUBJECT NUMBER" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="AGE" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SEX" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="LINK SENT" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="1" xr3:uid="{CD4CDB13-532F-4C56-A86A-6B439CF29546}" name="EXPERIMENT COMPLETED" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{5B371E51-03B6-41D4-90E0-50994B74D049}" name="TOTAL DURATION (minutes)" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{9E08D108-5F48-4257-A8B1-A9E4D6B05F3D}" name="TUTORIAL DURATION (minutes)" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="COMMENTS" dataDxfId="3" totalsRowDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella_Elenco_inventario" displayName="Tabella_Elenco_inventario" ref="B1:J26" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="B1:J26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="9">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SUBJECT NUMBER" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="AGE" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SEX" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="LINK SENT" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{CD4CDB13-532F-4C56-A86A-6B439CF29546}" name="EXPERIMENT COMPLETED" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{5B371E51-03B6-41D4-90E0-50994B74D049}" name="TOTAL DURATION (minutes)" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{6EA331DF-5C53-4D0C-8035-1EE65DB2A8DE}" name="AVERAGE BLOCK DURATION (minutes)" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{9E08D108-5F48-4257-A8B1-A9E4D6B05F3D}" name="TUTORIAL DURATION (minutes)" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="COMMENTS" dataDxfId="5" totalsRowDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="Tabella Aziendale" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1708,10 +1750,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:I14"/>
+  <dimension ref="B1:J14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1723,13 +1765,14 @@
     <col min="5" max="5" width="8.08984375" style="7" customWidth="1"/>
     <col min="6" max="6" width="11.81640625" style="7" customWidth="1"/>
     <col min="7" max="7" width="11.26953125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="13.6328125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="117.08984375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="1.81640625" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.81640625" style="2"/>
+    <col min="8" max="8" width="16.08984375" style="10" customWidth="1"/>
+    <col min="9" max="9" width="13.6328125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="117.08984375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="1.81640625" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:10" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1749,13 +1792,16 @@
         <v>9</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:9" ht="49.8" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" ht="49.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1">
         <v>1</v>
       </c>
@@ -1775,13 +1821,16 @@
         <v>27</v>
       </c>
       <c r="H2" s="12">
+        <v>3.4</v>
+      </c>
+      <c r="I2" s="12">
         <v>11</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>14</v>
+      <c r="J2" s="8" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>2</v>
       </c>
@@ -1801,13 +1850,16 @@
         <v>30</v>
       </c>
       <c r="H3" s="12">
+        <v>3.95</v>
+      </c>
+      <c r="I3" s="12">
         <v>13</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>17</v>
+      <c r="J3" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1">
         <v>3</v>
       </c>
@@ -1827,13 +1879,16 @@
         <v>18</v>
       </c>
       <c r="H4" s="12">
+        <v>1.36</v>
+      </c>
+      <c r="I4" s="12">
         <v>12</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>15</v>
+      <c r="J4" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="49.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1">
         <v>4</v>
       </c>
@@ -1853,13 +1908,16 @@
         <v>37</v>
       </c>
       <c r="H5" s="12">
+        <v>6.39</v>
+      </c>
+      <c r="I5" s="12">
         <v>10</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>16</v>
+      <c r="J5" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1">
         <v>5</v>
       </c>
@@ -1879,13 +1937,16 @@
         <v>20</v>
       </c>
       <c r="H6" s="12">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="I6" s="12">
         <v>9</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>23</v>
+      <c r="J6" s="8" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="64.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" ht="64.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1">
         <v>6</v>
       </c>
@@ -1905,13 +1966,16 @@
         <v>9</v>
       </c>
       <c r="H7" s="12">
+        <v>0.98</v>
+      </c>
+      <c r="I7" s="12">
         <v>5</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>18</v>
+      <c r="J7" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
         <v>7</v>
       </c>
@@ -1931,13 +1995,16 @@
         <v>6</v>
       </c>
       <c r="H8" s="12">
+        <v>0.63</v>
+      </c>
+      <c r="I8" s="12">
         <v>3</v>
       </c>
-      <c r="I8" s="8" t="s">
-        <v>19</v>
+      <c r="J8" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1">
         <v>8</v>
       </c>
@@ -1957,13 +2024,16 @@
         <v>31</v>
       </c>
       <c r="H9" s="12">
+        <v>4.53</v>
+      </c>
+      <c r="I9" s="12">
         <v>12</v>
       </c>
-      <c r="I9" s="8" t="s">
-        <v>20</v>
+      <c r="J9" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1">
         <v>9</v>
       </c>
@@ -1983,13 +2053,16 @@
         <v>23</v>
       </c>
       <c r="H10" s="12">
+        <v>2.57</v>
+      </c>
+      <c r="I10" s="12">
         <v>12</v>
       </c>
-      <c r="I10" s="8" t="s">
-        <v>21</v>
+      <c r="J10" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="201.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" ht="201.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1">
         <v>10</v>
       </c>
@@ -2006,28 +2079,55 @@
         <v>0.7631944444444444</v>
       </c>
       <c r="G11" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="13">
+        <v>4.21</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G13" s="10">
+        <f>AVERAGE(G2:G10)</f>
+        <v>22.333333333333332</v>
+      </c>
+      <c r="H13" s="10">
+        <f>AVERAGE(H2:H11)</f>
+        <v>3.0509999999999997</v>
+      </c>
+      <c r="I13" s="10">
+        <f xml:space="preserve"> AVERAGE(I2:I10)</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G14" s="10">
+        <f>_xlfn.STDEV.S(G3:G11)</f>
+        <v>10.793516572461451</v>
+      </c>
+      <c r="H14" s="10">
+        <f>_xlfn.STDEV.S(H2:H11)</f>
+        <v>1.8001694364698018</v>
+      </c>
+      <c r="I14" s="10">
+        <f xml:space="preserve"> _xlfn.STDEV.S(I3:I11)</f>
+        <v>3.6645015252516173</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="I13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="I14" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
-  <conditionalFormatting sqref="B2:I26">
+  <conditionalFormatting sqref="B17:J26 B15:G16 I15:J16 B2:J14">
     <cfRule type="expression" dxfId="1" priority="8">
       <formula>#REF!="Sì"</formula>
     </cfRule>
@@ -2038,8 +2138,8 @@
   <dataValidations xWindow="285" yWindow="468" count="5">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere l'ID inventario in questa colonna" sqref="B1" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il nome dell'articolo in questa colonna" sqref="C1" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la quantità in magazzino di ogni articolo in questa colonna" sqref="I1" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il prezzo unitario di ogni articolo in questa colonna" sqref="E1:H1" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere la quantità in magazzino di ogni articolo in questa colonna" sqref="J1" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere il prezzo unitario di ogni articolo in questa colonna" sqref="E1:I1" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Immettere una descrizione dell'articolo in questa colonna" sqref="D1" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2051,6 +2151,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DEEA25CC0A0AC24199CDC46C25B8B0BC" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3b47856d4cf355c0dacb39e1084d14f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6dc4bcd6-49db-4c07-9060-8acfc67cef9f" xmlns:ns3="fb0879af-3eba-417a-a55a-ffe6dcd6ca77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a845a615265fdb1f7b12cc65ac20ecbd" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2258,25 +2376,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1227E31-123E-44EE-A422-2705DF3A5917}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2294,22 +2412,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>